<commit_message>
fix agg data issues
</commit_message>
<xml_diff>
--- a/files/bdAfiliados.xlsx
+++ b/files/bdAfiliados.xlsx
@@ -666,7 +666,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ebb81f2b-007f-4262-8b9d-5449bed93942/Contrato%20Laura.docx%20-%20Clicksign.pdf?expires_on=1648559561&amp;signature=yU9%2F%2FNJJXwjiya9QA%2B3ItPP9bI%2By025kqDs591xest8%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ebb81f2b-007f-4262-8b9d-5449bed93942/Contrato%20Laura.docx%20-%20Clicksign.pdf?expires_on=1648599380&amp;signature=g4t92KqiRLDSv5pIf3Cq72HFDX5J6BaL%2BaTwgWaDUnQ%3D"]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -940,7 +940,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ecc62a90-29b6-447c-9058-53b38f2a7faf/Contrato%20Gabriel.docx%20-%20Clicksign.pdf?expires_on=1648559561&amp;signature=yAnOrNOUdQibWFzxid%2FhdfGECaFXfWjTJwUQKAJw3CE%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ecc62a90-29b6-447c-9058-53b38f2a7faf/Contrato%20Gabriel.docx%20-%20Clicksign.pdf?expires_on=1648599380&amp;signature=JLkomHwqOdoY1S8zRFF%2FFi5QWW8ArkMUXmPzFwS2okI%3D"]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/d8d41087-022b-43a9-b3a7-c2767d22ee32/Contrato%20Nicolas%20%2B%20Tati%202.docx%20-%20Clicksign.pdf?expires_on=1648559561&amp;signature=BT9ee%2FrKcyj17Bzd%2FoqmkEFzY1ZIEKNFhe%2F5mPBsxK4%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/d8d41087-022b-43a9-b3a7-c2767d22ee32/Contrato%20Nicolas%20%2B%20Tati%202.docx%20-%20Clicksign.pdf?expires_on=1648599380&amp;signature=9qpZKDD3Kufi0xzg%2FKSqCiSLnpgXyAVqOGpaFCLrLho%3D"]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/1d4e7e1b-6181-4d68-9f4c-2af92343a1b0/Contrato%20assinado%20J%C3%A9ssica.pdf?expires_on=1648559561&amp;signature=XvgPKF8%2Fhh%2FrdY6cjg6NDCXYhRowayW7jPokSkRnjRo%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/1d4e7e1b-6181-4d68-9f4c-2af92343a1b0/Contrato%20assinado%20J%C3%A9ssica.pdf?expires_on=1648599380&amp;signature=B21fxsUHieB%2ByWqC6VSBp0eIdaKNZa0RTAz1KUo%2BQg8%3D"]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/f034a244-7db2-4690-b6dd-a0e136e82f13/Contrato%20assinado%20Diogo.pdf?expires_on=1648559561&amp;signature=udu8C8TcGeFw8egBndZ8eJhmUW8II9hFH3OeAwz5lBY%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/f034a244-7db2-4690-b6dd-a0e136e82f13/Contrato%20assinado%20Diogo.pdf?expires_on=1648599380&amp;signature=%2F45v5Q%2BREAb3nlLdO7l8RB%2FbYiBtXNjqeaqyD9%2BVOVk%3D"]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/f7a08a78-1cd3-4fd4-9e0f-8ffef864bc64/0c6b523f-688c-4083-8149-42b1e8bad674.pdf?expires_on=1648559561&amp;signature=7O%2FgO7owus7M%2B117qQMhP8LkGAq8fwVQHfO%2FXHGbfro%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/f7a08a78-1cd3-4fd4-9e0f-8ffef864bc64/0c6b523f-688c-4083-8149-42b1e8bad674.pdf?expires_on=1648599380&amp;signature=PbU4L1PhCWzZNstKKRzYjqRqEMmkZBEZjM82MQiNLhI%3D"]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ebe95716-517c-4801-90b1-12b470a87eba/d7f66983-f556-4e7a-ab80-c6a9091bd63c.pdf?expires_on=1648559561&amp;signature=kGX8ue0%2FX8AlQ9GvWj1JBWNJ%2BTCR%2FSB4pkZGb49WRBQ%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/ebe95716-517c-4801-90b1-12b470a87eba/d7f66983-f556-4e7a-ab80-c6a9091bd63c.pdf?expires_on=1648599380&amp;signature=iCEmj8S%2BfMJb3guQsqjtIRczlL%2BGaKOiJLwzI3Z45Do%3D"]</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/4701c047-3d98-4603-9e08-4e07637a1e2b/283e96ef-2df5-4fbd-866a-017ca2a54b46.pdf?expires_on=1648559561&amp;signature=Z2bWPts06JpkQkFFAGD8%2BsIK%2Bla2j8ohcAu59xEfcs0%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/4701c047-3d98-4603-9e08-4e07637a1e2b/283e96ef-2df5-4fbd-866a-017ca2a54b46.pdf?expires_on=1648599380&amp;signature=gUjOryNotM%2BDr%2BSYdYokUYwDVxDSUTx7J325eukptJ4%3D"]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/b04664f2-a9f4-4126-908b-fcf7d0d927af/0abc913e-411a-432f-a576-8c8ac06efafe.pdf?expires_on=1648559561&amp;signature=Q%2FCMFZp3uOPjcf60YBXln5K5eKMqOtNOwF5LE1rP3BY%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/b04664f2-a9f4-4126-908b-fcf7d0d927af/0abc913e-411a-432f-a576-8c8ac06efafe.pdf?expires_on=1648599380&amp;signature=zG58mIyHoZxoSichclvRhcUjVMg4tB%2BsjEZZDYM4M1w%3D"]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/04631026-fd1b-4df0-922e-b4ae8244b68b/Karinad40db3de-88e0-4ea8-a807-4d8c1b474c99.pdf?expires_on=1648559561&amp;signature=COUhdGK9nqElQHdoAJLBLDxDIThJfnDh9AonAt2D%2Bkg%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/04631026-fd1b-4df0-922e-b4ae8244b68b/Karinad40db3de-88e0-4ea8-a807-4d8c1b474c99.pdf?expires_on=1648599380&amp;signature=HENxRlHflDPnMtvysRUnAFw7WCczsyJfZkGvW8TifEI%3D"]</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/0d70b51d-9526-4d01-952e-52987225f2fe/ec5fd910-8712-4b2f-8ec0-5852e10605ae.pdf?expires_on=1648559561&amp;signature=iZXMriWySSd1FpZN6ofYgFGwBPzGeqKaw%2F5uzgIgLWA%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/0d70b51d-9526-4d01-952e-52987225f2fe/ec5fd910-8712-4b2f-8ec0-5852e10605ae.pdf?expires_on=1648599380&amp;signature=uyH1ZPiBFmc3huEAgVOn1QM6BReuMf8t9GcuiFFOK4E%3D"]</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/a4645a7b-0477-4878-82bc-8975dd3c019a/0be53e8a-b7e8-41b8-b3e9-db52641599cd.pdf?expires_on=1648559561&amp;signature=oB%2B4RlDQqYJ%2FH4hyXqaqIm5mxX%2BIKOnV42ra85vGel4%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/a4645a7b-0477-4878-82bc-8975dd3c019a/0be53e8a-b7e8-41b8-b3e9-db52641599cd.pdf?expires_on=1648599380&amp;signature=kYbhEkRLveKNAmY6zs357be1PdlOdZEy1oXNPi%2Bqnps%3D"]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2773,7 +2773,7 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
         <is>
-          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/1cd35f18-267f-4a52-a0a4-a8fcc3a4550b/4243707f-fa7b-480f-9cb8-1b532548f132.pdf?expires_on=1648559561&amp;signature=KLX2UsyoSbYHyp56t7V%2BjQPuqQNGMVnx4wsGzWJ0%2FNY%3D"]</t>
+          <t>["https://app-storage-service.pipefy.com/v1/signed/uploads/1cd35f18-267f-4a52-a0a4-a8fcc3a4550b/4243707f-fa7b-480f-9cb8-1b532548f132.pdf?expires_on=1648599380&amp;signature=VsucxZJdbykXaVjRP5rq3FjURmn1s9N%2BKSBtl6E7knI%3D"]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>